<commit_message>
[#641] Read orientation: call flattentool.unflatent with metatab_vertical_orientation (ie vertical headings at column 0)
</commit_message>
<xml_diff>
--- a/cove_ocds/fixtures/tenders_releases_2_releases_with_metatab_version_1_1_extensions.xlsx
+++ b/cove_ocds/fixtures/tenders_releases_2_releases_with_metatab_version_1_1_extensions.xlsx
@@ -166,7 +166,7 @@
     <t xml:space="preserve">extensions</t>
   </si>
   <si>
-    <t xml:space="preserve">https://raw.githubusercontent.com/open-contracting/ocds_metrics_extension/master/extension.json; https://raw.githubusercontent.com/open-contracting/ocds_extension_parties/master/extension.json;   https://raw.githubusercontent.com/open-contracting/ocds_partyDetails_scale_extension/master/extension.json</t>
+    <t xml:space="preserve">https://raw.githubusercontent.com/open-contracting/ocds_metrics_extension/master/extension.json;https://raw.githubusercontent.com/open-contracting/ocds_extension_parties/master/extension.json;https://raw.githubusercontent.com/open-contracting/ocds_partyDetails_scale_extension/master/extension.json</t>
   </si>
 </sst>
 </file>
@@ -270,13 +270,13 @@
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="15.8016194331984"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="17.3238866396761"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -405,16 +405,16 @@
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8016194331984"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.8906882591093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="58.9352226720648"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="15.8016194331984"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.3238866396761"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.5101214574899"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.5587044534413"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="17.3238866396761"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -588,16 +588,16 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8016194331984"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.748987854251"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.8906882591093"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="15.8016194331984"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.3238866396761"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.7975708502024"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.3279352226721"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="17.3238866396761"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -685,41 +685,38 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.9473684210526"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="178.437246963563"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.9028340080972"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="37.3279352226721"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="18.9473684210526"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.3481781376518"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="244.708502024291"/>
+    <col collapsed="false" hidden="true" max="4" min="3" style="1" width="0"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="20.668016194332"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="n">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="0" t="s">
         <v>47</v>
       </c>
     </row>
+    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://raw.githubusercontent.com/open-contracting/ocds_metrics_extension/master/extension.json; https://raw.githubusercontent.com/open-contracting/ocds_extension_parties/master/extension.json;   https://raw.githubusercontent.com/open-contracting/ocds_partyDetails_scale_extension/master/extension.json"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>